<commit_message>
changed code to store data in mongo. Trying to figure out how to query
</commit_message>
<xml_diff>
--- a/presentation_excel/fp_master.xlsx
+++ b/presentation_excel/fp_master.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="50">
+  <si>
+    <t>Date</t>
+  </si>
   <si>
     <t>Average Service rating</t>
   </si>
@@ -62,70 +65,25 @@
     <t>comments</t>
   </si>
   <si>
+    <t>Unnamed: 13</t>
+  </si>
+  <si>
     <t>y</t>
   </si>
   <si>
     <t>n</t>
   </si>
   <si>
+    <t>Ticket price was lower than expected</t>
+  </si>
+  <si>
     <t>Ticket Matched Expected Price</t>
   </si>
   <si>
     <t>Price was not marked on ticket</t>
   </si>
   <si>
-    <t>Ticket price was lower than expected</t>
-  </si>
-  <si>
     <t>Ticket price was more than expected</t>
-  </si>
-  <si>
-    <t>Nice Place</t>
-  </si>
-  <si>
-    <t>Great Job!</t>
-  </si>
-  <si>
-    <t>Great experience - glad you're here</t>
-  </si>
-  <si>
-    <t>Full menu after lunch rush and dessert all day :) Excellent</t>
-  </si>
-  <si>
-    <t>Thanks for all the vegetarian food!</t>
-  </si>
-  <si>
-    <t>An espresso bar would be nice.</t>
-  </si>
-  <si>
-    <t>I will be back ! :)</t>
-  </si>
-  <si>
-    <t>5 being best experience possible. Overall great. Thank you</t>
-  </si>
-  <si>
-    <t>We'll be back !!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We'll will see you again </t>
-  </si>
-  <si>
-    <t>Thank you Michael !!</t>
-  </si>
-  <si>
-    <t>More gluten free/vegan options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Be more cognisant of clearing plates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Appetizer steak still sitting on table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Replace silverware instead of asking guest to keep it</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Return to table after entrée to check on food quality</t>
   </si>
   <si>
     <t>The price point is reasonable enough to keep people coming back.</t>
@@ -564,13 +522,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -586,45 +544,54 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
         <v>4.444444444444445</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>4.192307692307693</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>4.555555555555555</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>4.333333333333333</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>4.222222222222222</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>4.514705882352941</v>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>4.283582089552239</v>
+        <v>4.444444444444445</v>
       </c>
       <c r="D3">
-        <v>4.602941176470588</v>
+        <v>4.192307692307693</v>
       </c>
       <c r="E3">
-        <v>4.397058823529412</v>
+        <v>4.555555555555555</v>
       </c>
       <c r="F3">
-        <v>4.308823529411764</v>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="G3">
+        <v>4.222222222222222</v>
       </c>
     </row>
   </sheetData>
@@ -634,68 +601,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -703,57 +673,57 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F3">
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -773,45 +743,45 @@
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -819,36 +789,36 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -860,16 +830,16 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -880,141 +850,141 @@
         <v>5</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F10">
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <v>5</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11">
         <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H12" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1022,7 +992,7 @@
         <v>5</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -1031,27 +1001,27 @@
         <v>5</v>
       </c>
       <c r="F14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H14" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -1060,19 +1030,19 @@
         <v>5</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1092,13 +1062,13 @@
         <v>5</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H16" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1106,7 +1076,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -1115,19 +1085,19 @@
         <v>5</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F17">
         <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H17" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1150,13 +1120,13 @@
         <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1176,16 +1146,16 @@
         <v>5</v>
       </c>
       <c r="F19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H19" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1196,25 +1166,25 @@
         <v>5</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G20" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I20" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1225,25 +1195,25 @@
         <v>5</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21">
         <v>5</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21">
         <v>5</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H21" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1251,28 +1221,28 @@
         <v>20</v>
       </c>
       <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22">
         <v>1</v>
       </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>5</v>
-      </c>
-      <c r="E22">
-        <v>3</v>
-      </c>
-      <c r="F22">
-        <v>5</v>
-      </c>
       <c r="G22" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H22" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1283,25 +1253,25 @@
         <v>5</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D23">
         <v>5</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G23" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H23" t="s">
         <v>20</v>
       </c>
       <c r="I23" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1309,10 +1279,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D24">
         <v>5</v>
@@ -1321,16 +1291,16 @@
         <v>5</v>
       </c>
       <c r="F24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H24" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1341,25 +1311,25 @@
         <v>5</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G25" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H25" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I25" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1370,25 +1340,25 @@
         <v>4</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G26" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H26" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1396,28 +1366,25 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D27">
         <v>5</v>
       </c>
       <c r="E27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F27">
         <v>5</v>
       </c>
       <c r="G27" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I27" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1425,28 +1392,22 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G28" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I28" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1454,7 +1415,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C29">
         <v>5</v>
@@ -1463,19 +1424,19 @@
         <v>5</v>
       </c>
       <c r="E29">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F29">
         <v>5</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H29" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I29" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1486,7 +1447,7 @@
         <v>5</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D30">
         <v>5</v>
@@ -1495,16 +1456,16 @@
         <v>5</v>
       </c>
       <c r="F30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I30" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1515,7 +1476,7 @@
         <v>5</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D31">
         <v>5</v>
@@ -1524,16 +1485,16 @@
         <v>5</v>
       </c>
       <c r="F31">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G31" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H31" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I31" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1556,13 +1517,13 @@
         <v>5</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H32" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I32" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1570,28 +1531,28 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>5</v>
       </c>
       <c r="E33">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F33">
         <v>5</v>
       </c>
       <c r="G33" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H33" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I33" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1602,25 +1563,25 @@
         <v>5</v>
       </c>
       <c r="C34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D34">
         <v>5</v>
       </c>
       <c r="E34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G34" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H34" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I34" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1628,10 +1589,10 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D35">
         <v>5</v>
@@ -1643,13 +1604,13 @@
         <v>5</v>
       </c>
       <c r="G35" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H35" t="s">
         <v>20</v>
       </c>
       <c r="I35" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1660,25 +1621,25 @@
         <v>5</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G36" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H36" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I36" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1686,28 +1647,28 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>4</v>
       </c>
       <c r="D37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E37">
         <v>4</v>
       </c>
       <c r="F37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G37" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H37" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I37" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1715,28 +1676,28 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D38">
         <v>5</v>
       </c>
       <c r="E38">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H38" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I38" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1744,28 +1705,28 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D39">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E39">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F39">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G39" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H39" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I39" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1773,7 +1734,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <v>5</v>
@@ -1782,19 +1743,19 @@
         <v>5</v>
       </c>
       <c r="E40">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F40">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G40" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H40" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I40" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1805,25 +1766,25 @@
         <v>5</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D41">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E41">
         <v>5</v>
       </c>
       <c r="F41">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G41" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H41" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I41" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1831,28 +1792,28 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E42">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F42">
         <v>3</v>
       </c>
       <c r="G42" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H42" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I42" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1875,10 +1836,10 @@
         <v>5</v>
       </c>
       <c r="G43" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H43" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I43" t="s">
         <v>37</v>
@@ -1901,13 +1862,13 @@
         <v>5</v>
       </c>
       <c r="F44">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G44" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H44" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I44" t="s">
         <v>38</v>
@@ -1933,10 +1894,10 @@
         <v>5</v>
       </c>
       <c r="G45" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H45" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I45" t="s">
         <v>39</v>
@@ -1962,10 +1923,10 @@
         <v>5</v>
       </c>
       <c r="G46" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H46" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I46" t="s">
         <v>40</v>
@@ -1976,25 +1937,25 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E47">
         <v>3</v>
       </c>
       <c r="F47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H47" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I47" t="s">
         <v>41</v>
@@ -2017,13 +1978,13 @@
         <v>4</v>
       </c>
       <c r="F48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G48" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H48" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I48" t="s">
         <v>42</v>
@@ -2034,10 +1995,10 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D49">
         <v>5</v>
@@ -2046,13 +2007,13 @@
         <v>5</v>
       </c>
       <c r="F49">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H49" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I49" t="s">
         <v>43</v>
@@ -2069,19 +2030,19 @@
         <v>5</v>
       </c>
       <c r="D50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G50" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H50" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I50" t="s">
         <v>44</v>
@@ -2092,25 +2053,25 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E51">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F51">
         <v>4</v>
       </c>
       <c r="G51" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H51" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I51" t="s">
         <v>45</v>
@@ -2121,22 +2082,22 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C52">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D52">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F52">
         <v>5</v>
       </c>
       <c r="G52" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H52" t="s">
         <v>20</v>
@@ -2150,25 +2111,25 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F53">
         <v>3</v>
       </c>
       <c r="G53" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H53" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I53" t="s">
         <v>47</v>
@@ -2179,7 +2140,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C54">
         <v>5</v>
@@ -2188,15 +2149,12 @@
         <v>5</v>
       </c>
       <c r="E54">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F54">
         <v>5</v>
       </c>
       <c r="G54" t="s">
-        <v>15</v>
-      </c>
-      <c r="H54" t="s">
         <v>17</v>
       </c>
       <c r="I54" t="s">
@@ -2208,425 +2166,22 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>5</v>
-      </c>
-      <c r="C55">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D55">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E55">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F55">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G55" t="s">
-        <v>15</v>
-      </c>
-      <c r="H55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I55" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="1">
-        <v>54</v>
-      </c>
-      <c r="B56">
-        <v>5</v>
-      </c>
-      <c r="C56">
-        <v>4</v>
-      </c>
-      <c r="D56">
-        <v>5</v>
-      </c>
-      <c r="E56">
-        <v>5</v>
-      </c>
-      <c r="F56">
-        <v>3</v>
-      </c>
-      <c r="G56" t="s">
-        <v>15</v>
-      </c>
-      <c r="H56" t="s">
-        <v>17</v>
-      </c>
-      <c r="I56" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="1">
-        <v>55</v>
-      </c>
-      <c r="B57">
-        <v>5</v>
-      </c>
-      <c r="C57">
-        <v>5</v>
-      </c>
-      <c r="D57">
-        <v>5</v>
-      </c>
-      <c r="E57">
-        <v>5</v>
-      </c>
-      <c r="F57">
-        <v>5</v>
-      </c>
-      <c r="G57" t="s">
-        <v>15</v>
-      </c>
-      <c r="H57" t="s">
-        <v>17</v>
-      </c>
-      <c r="I57" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="1">
-        <v>56</v>
-      </c>
-      <c r="B58">
-        <v>5</v>
-      </c>
-      <c r="C58">
-        <v>5</v>
-      </c>
-      <c r="D58">
-        <v>5</v>
-      </c>
-      <c r="E58">
-        <v>5</v>
-      </c>
-      <c r="F58">
-        <v>5</v>
-      </c>
-      <c r="G58" t="s">
-        <v>15</v>
-      </c>
-      <c r="H58" t="s">
-        <v>17</v>
-      </c>
-      <c r="I58" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="1">
-        <v>57</v>
-      </c>
-      <c r="B59">
-        <v>5</v>
-      </c>
-      <c r="C59">
-        <v>5</v>
-      </c>
-      <c r="D59">
-        <v>5</v>
-      </c>
-      <c r="E59">
-        <v>5</v>
-      </c>
-      <c r="F59">
-        <v>5</v>
-      </c>
-      <c r="G59" t="s">
-        <v>15</v>
-      </c>
-      <c r="H59" t="s">
-        <v>18</v>
-      </c>
-      <c r="I59" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="1">
-        <v>58</v>
-      </c>
-      <c r="B60">
-        <v>5</v>
-      </c>
-      <c r="C60">
-        <v>5</v>
-      </c>
-      <c r="D60">
-        <v>5</v>
-      </c>
-      <c r="E60">
-        <v>5</v>
-      </c>
-      <c r="F60">
-        <v>5</v>
-      </c>
-      <c r="G60" t="s">
-        <v>15</v>
-      </c>
-      <c r="H60" t="s">
-        <v>20</v>
-      </c>
-      <c r="I60" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="1">
-        <v>59</v>
-      </c>
-      <c r="B61">
-        <v>5</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-      <c r="D61">
-        <v>3</v>
-      </c>
-      <c r="E61">
-        <v>3</v>
-      </c>
-      <c r="F61">
-        <v>2</v>
-      </c>
-      <c r="G61" t="s">
-        <v>15</v>
-      </c>
-      <c r="H61" t="s">
-        <v>17</v>
-      </c>
-      <c r="I61" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="1">
-        <v>60</v>
-      </c>
-      <c r="B62">
-        <v>5</v>
-      </c>
-      <c r="C62">
-        <v>4</v>
-      </c>
-      <c r="D62">
-        <v>5</v>
-      </c>
-      <c r="E62">
-        <v>4</v>
-      </c>
-      <c r="F62">
-        <v>5</v>
-      </c>
-      <c r="G62" t="s">
-        <v>15</v>
-      </c>
-      <c r="H62" t="s">
-        <v>18</v>
-      </c>
-      <c r="I62" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="1">
-        <v>61</v>
-      </c>
-      <c r="B63">
-        <v>5</v>
-      </c>
-      <c r="C63">
-        <v>5</v>
-      </c>
-      <c r="D63">
-        <v>5</v>
-      </c>
-      <c r="E63">
-        <v>5</v>
-      </c>
-      <c r="F63">
-        <v>1</v>
-      </c>
-      <c r="G63" t="s">
-        <v>16</v>
-      </c>
-      <c r="H63" t="s">
-        <v>17</v>
-      </c>
-      <c r="I63" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="1">
-        <v>62</v>
-      </c>
-      <c r="B64">
-        <v>5</v>
-      </c>
-      <c r="C64">
-        <v>5</v>
-      </c>
-      <c r="D64">
-        <v>5</v>
-      </c>
-      <c r="E64">
-        <v>5</v>
-      </c>
-      <c r="F64">
-        <v>5</v>
-      </c>
-      <c r="G64" t="s">
-        <v>15</v>
-      </c>
-      <c r="H64" t="s">
-        <v>17</v>
-      </c>
-      <c r="I64" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
-      <c r="A65" s="1">
-        <v>63</v>
-      </c>
-      <c r="B65">
-        <v>5</v>
-      </c>
-      <c r="C65">
-        <v>5</v>
-      </c>
-      <c r="D65">
-        <v>5</v>
-      </c>
-      <c r="E65">
-        <v>5</v>
-      </c>
-      <c r="F65">
-        <v>4</v>
-      </c>
-      <c r="G65" t="s">
-        <v>15</v>
-      </c>
-      <c r="H65" t="s">
-        <v>17</v>
-      </c>
-      <c r="I65" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
-      <c r="A66" s="1">
-        <v>64</v>
-      </c>
-      <c r="B66">
-        <v>5</v>
-      </c>
-      <c r="C66">
-        <v>3</v>
-      </c>
-      <c r="D66">
-        <v>3</v>
-      </c>
-      <c r="E66">
-        <v>5</v>
-      </c>
-      <c r="F66">
-        <v>5</v>
-      </c>
-      <c r="G66" t="s">
-        <v>15</v>
-      </c>
-      <c r="H66" t="s">
-        <v>17</v>
-      </c>
-      <c r="I66" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
-      <c r="A67" s="1">
-        <v>65</v>
-      </c>
-      <c r="B67">
-        <v>4</v>
-      </c>
-      <c r="C67">
-        <v>5</v>
-      </c>
-      <c r="D67">
-        <v>3</v>
-      </c>
-      <c r="E67">
-        <v>3</v>
-      </c>
-      <c r="F67">
-        <v>3</v>
-      </c>
-      <c r="G67" t="s">
-        <v>16</v>
-      </c>
-      <c r="H67" t="s">
-        <v>18</v>
-      </c>
-      <c r="I67" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
-      <c r="A68" s="1">
-        <v>66</v>
-      </c>
-      <c r="B68">
-        <v>5</v>
-      </c>
-      <c r="C68">
-        <v>5</v>
-      </c>
-      <c r="D68">
-        <v>5</v>
-      </c>
-      <c r="E68">
-        <v>5</v>
-      </c>
-      <c r="F68">
-        <v>5</v>
-      </c>
-      <c r="G68" t="s">
-        <v>15</v>
-      </c>
-      <c r="I68" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
-      <c r="A69" s="1">
-        <v>67</v>
-      </c>
-      <c r="B69">
-        <v>3</v>
-      </c>
-      <c r="D69">
-        <v>4</v>
-      </c>
-      <c r="E69">
-        <v>4</v>
-      </c>
-      <c r="F69">
-        <v>4</v>
-      </c>
-      <c r="G69" t="s">
-        <v>15</v>
-      </c>
-      <c r="I69" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>